<commit_message>
fix cleanall issue and germ yr
</commit_message>
<xml_diff>
--- a/data/egret_SS.xlsx
+++ b/data/egret_SS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/egret/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B3FEBF-28BC-4649-AF9B-67C3F9F3796F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4073D46-C1B3-E24F-A255-DA906D92B4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35140" yWindow="3480" windowWidth="33400" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="155">
   <si>
     <t>datasetID</t>
   </si>
@@ -489,9 +489,6 @@
   </si>
   <si>
     <t xml:space="preserve">number of days germination monitored -- negative values should be used if germination occurs prior to the start of the experiment </t>
-  </si>
-  <si>
-    <t>germ.tim.zero</t>
   </si>
   <si>
     <t>The zero point germination is measured relative to - "end cold strat" - other options include "unknown", "start emergence, X days after end cold strat", "other, end of treatment X"</t>
@@ -1418,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1948,10 +1945,10 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" t="s">
         <v>152</v>
-      </c>
-      <c r="B70" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1967,7 +1964,7 @@
         <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1990,8 +1987,8 @@
   <dimension ref="A1:AS382"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F116" sqref="F116"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2129,7 +2126,7 @@
         <v>34</v>
       </c>
       <c r="AQ1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AR1" t="s">
         <v>35</v>

</xml_diff>